<commit_message>
Regresión Lasso en python
Dos modelos ya realizados
</commit_message>
<xml_diff>
--- a/Python/Datos/df_series.xlsx
+++ b/Python/Datos/df_series.xlsx
@@ -1,24 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Proyecto4-riesgo-de-liquidez\Python\Datos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895EF2B4-A7C1-4720-AD21-A69B030F05D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Datos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>TIIE</t>
+  </si>
+  <si>
+    <t>FIX</t>
+  </si>
+  <si>
+    <t>Base_Monetaria</t>
+  </si>
+  <si>
+    <t>Remesas_Familiares</t>
+  </si>
+  <si>
+    <t>INPC</t>
+  </si>
+  <si>
+    <t>Costo_Captacion</t>
+  </si>
+  <si>
+    <t>Agregados_Monetarios</t>
+  </si>
+  <si>
+    <t>Activos_Financieros</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,13 +105,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -111,7 +157,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -145,6 +191,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -179,9 +226,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -354,64 +402,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Fecha</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>TIIE</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>FIX</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Base_Monetaria</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Remesas_Familiares</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>INPC</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Costo_Captacion</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Agregados_Monetarios</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Activos_Financieros</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43800</v>
       </c>
@@ -419,7 +451,7 @@
         <v>7.7</v>
       </c>
       <c r="C2">
-        <v>19.1071</v>
+        <v>19.107099999999999</v>
       </c>
       <c r="D2">
         <v>1742474.7</v>
@@ -428,7 +460,7 @@
         <v>3197.7419</v>
       </c>
       <c r="F2">
-        <v>0.5600000000000001</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G2">
         <v>6.77</v>
@@ -440,7 +472,7 @@
         <v>142186457.44</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43831</v>
       </c>
@@ -448,13 +480,13 @@
         <v>7.53</v>
       </c>
       <c r="C3">
-        <v>18.804</v>
+        <v>18.803999999999998</v>
       </c>
       <c r="D3">
         <v>1697686.8</v>
       </c>
       <c r="E3">
-        <v>2676.6263</v>
+        <v>2676.6262999999999</v>
       </c>
       <c r="F3">
         <v>0.48</v>
@@ -463,13 +495,13 @@
         <v>6.61</v>
       </c>
       <c r="H3">
-        <v>132615054.6</v>
+        <v>132615054.59999999</v>
       </c>
       <c r="I3">
-        <v>142470720.2</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>142470720.19999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43862</v>
       </c>
@@ -483,7 +515,7 @@
         <v>1670342.9</v>
       </c>
       <c r="E4">
-        <v>2803.4988</v>
+        <v>2803.4987999999998</v>
       </c>
       <c r="F4">
         <v>0.42</v>
@@ -495,10 +527,10 @@
         <v>133870970.48</v>
       </c>
       <c r="I4">
-        <v>143202721.6</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>143202721.59999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43891</v>
       </c>
@@ -506,13 +538,13 @@
         <v>7.1</v>
       </c>
       <c r="C5">
-        <v>22.3784</v>
+        <v>22.378399999999999</v>
       </c>
       <c r="D5">
         <v>1770527.8</v>
       </c>
       <c r="E5">
-        <v>4147.1146</v>
+        <v>4147.1145999999999</v>
       </c>
       <c r="F5">
         <v>-0.05</v>
@@ -524,10 +556,10 @@
         <v>135165044.47</v>
       </c>
       <c r="I5">
-        <v>145447940.58</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>145447940.58000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43922</v>
       </c>
@@ -535,7 +567,7 @@
         <v>6.54</v>
       </c>
       <c r="C6">
-        <v>24.2658</v>
+        <v>24.265799999999999</v>
       </c>
       <c r="D6">
         <v>1791788.6</v>
@@ -556,7 +588,7 @@
         <v>145174793.28</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43952</v>
       </c>
@@ -564,13 +596,13 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>23.423</v>
+        <v>23.422999999999998</v>
       </c>
       <c r="D7">
         <v>1850823.7</v>
       </c>
       <c r="E7">
-        <v>3541.8263</v>
+        <v>3541.8263000000002</v>
       </c>
       <c r="F7">
         <v>0.38</v>
@@ -585,7 +617,7 @@
         <v>147421919.03</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43983</v>
       </c>
@@ -593,16 +625,16 @@
         <v>5.65</v>
       </c>
       <c r="C8">
-        <v>22.299</v>
+        <v>22.298999999999999</v>
       </c>
       <c r="D8">
         <v>1857091.9</v>
       </c>
       <c r="E8">
-        <v>3630.6225</v>
+        <v>3630.6224999999999</v>
       </c>
       <c r="F8">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G8">
         <v>5.23</v>
@@ -611,10 +643,10 @@
         <v>139145368.37</v>
       </c>
       <c r="I8">
-        <v>147159048.32</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>147159048.31999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44013</v>
       </c>
@@ -622,13 +654,13 @@
         <v>5.23</v>
       </c>
       <c r="C9">
-        <v>22.4033</v>
+        <v>22.403300000000002</v>
       </c>
       <c r="D9">
         <v>1914661.9</v>
       </c>
       <c r="E9">
-        <v>3629.1537</v>
+        <v>3629.1536999999998</v>
       </c>
       <c r="F9">
         <v>0.66</v>
@@ -640,10 +672,10 @@
         <v>141328981.44</v>
       </c>
       <c r="I9">
-        <v>150326476.64</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>150326476.63999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44044</v>
       </c>
@@ -657,7 +689,7 @@
         <v>1914937.7</v>
       </c>
       <c r="E10">
-        <v>3654.1707</v>
+        <v>3654.1707000000001</v>
       </c>
       <c r="F10">
         <v>0.39</v>
@@ -669,10 +701,10 @@
         <v>143207284.56</v>
       </c>
       <c r="I10">
-        <v>151489310.67</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>151489310.66999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44075</v>
       </c>
@@ -680,13 +712,13 @@
         <v>4.72</v>
       </c>
       <c r="C11">
-        <v>21.681</v>
+        <v>21.681000000000001</v>
       </c>
       <c r="D11">
         <v>1898295.5</v>
       </c>
       <c r="E11">
-        <v>3673.8419</v>
+        <v>3673.8418999999999</v>
       </c>
       <c r="F11">
         <v>0.23</v>
@@ -698,10 +730,10 @@
         <v>144913654.41</v>
       </c>
       <c r="I11">
-        <v>155091165.23</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>155091165.22999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44105</v>
       </c>
@@ -709,28 +741,28 @@
         <v>4.53</v>
       </c>
       <c r="C12">
-        <v>21.2705</v>
+        <v>21.270499999999998</v>
       </c>
       <c r="D12">
         <v>1920444.2</v>
       </c>
       <c r="E12">
-        <v>3715.2525</v>
+        <v>3715.2525000000001</v>
       </c>
       <c r="F12">
         <v>0.61</v>
       </c>
       <c r="G12">
-        <v>4.14</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="H12">
-        <v>145566764.02</v>
+        <v>145566764.02000001</v>
       </c>
       <c r="I12">
-        <v>155281437.6</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>155281437.59999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44136</v>
       </c>
@@ -738,13 +770,13 @@
         <v>4.5</v>
       </c>
       <c r="C13">
-        <v>20.3819</v>
+        <v>20.381900000000002</v>
       </c>
       <c r="D13">
         <v>1990505.5</v>
       </c>
       <c r="E13">
-        <v>3491.9473</v>
+        <v>3491.9472999999998</v>
       </c>
       <c r="F13">
         <v>0.08</v>
@@ -753,13 +785,13 @@
         <v>4.05</v>
       </c>
       <c r="H13">
-        <v>145766600.54</v>
+        <v>145766600.53999999</v>
       </c>
       <c r="I13">
-        <v>157047266.71</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>157047266.71000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44166</v>
       </c>
@@ -782,13 +814,13 @@
         <v>4.03</v>
       </c>
       <c r="H14">
-        <v>147441141.21</v>
+        <v>147441141.21000001</v>
       </c>
       <c r="I14">
-        <v>152675155.95</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>152675155.94999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44197</v>
       </c>
@@ -796,19 +828,19 @@
         <v>4.47</v>
       </c>
       <c r="C15">
-        <v>19.9215</v>
+        <v>19.921500000000002</v>
       </c>
       <c r="D15">
         <v>2101714</v>
       </c>
       <c r="E15">
-        <v>3392.8085</v>
+        <v>3392.8085000000001</v>
       </c>
       <c r="F15">
         <v>0.86</v>
       </c>
       <c r="G15">
-        <v>4.02</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="H15">
         <v>149347286.66</v>
@@ -817,21 +849,21 @@
         <v>150506134.59</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44228</v>
       </c>
       <c r="B16">
-        <v>4.36</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="C16">
-        <v>20.3097</v>
+        <v>20.309699999999999</v>
       </c>
       <c r="D16">
         <v>2088210.3</v>
       </c>
       <c r="E16">
-        <v>3264.1015</v>
+        <v>3264.1015000000002</v>
       </c>
       <c r="F16">
         <v>0.63</v>
@@ -840,13 +872,13 @@
         <v>3.94</v>
       </c>
       <c r="H16">
-        <v>150692817.96</v>
+        <v>150692817.96000001</v>
       </c>
       <c r="I16">
-        <v>150760434.89</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>150760434.88999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44256</v>
       </c>
@@ -854,13 +886,13 @@
         <v>4.28</v>
       </c>
       <c r="C17">
-        <v>20.7555</v>
+        <v>20.755500000000001</v>
       </c>
       <c r="D17">
-        <v>2178191.7</v>
+        <v>2178191.7000000002</v>
       </c>
       <c r="E17">
-        <v>4275.0937</v>
+        <v>4275.0937000000004</v>
       </c>
       <c r="F17">
         <v>0.83</v>
@@ -869,13 +901,13 @@
         <v>3.83</v>
       </c>
       <c r="H17">
-        <v>152496745.46</v>
+        <v>152496745.46000001</v>
       </c>
       <c r="I17">
         <v>154389303.59</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44287</v>
       </c>
@@ -889,7 +921,7 @@
         <v>2148400.1</v>
       </c>
       <c r="E18">
-        <v>4167.7596</v>
+        <v>4167.7596000000003</v>
       </c>
       <c r="F18">
         <v>0.33</v>
@@ -898,13 +930,13 @@
         <v>3.79</v>
       </c>
       <c r="H18">
-        <v>154209175.58</v>
+        <v>154209175.58000001</v>
       </c>
       <c r="I18">
-        <v>152332526.01</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>152332526.00999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44317</v>
       </c>
@@ -912,7 +944,7 @@
         <v>4.29</v>
       </c>
       <c r="C19">
-        <v>19.9631</v>
+        <v>19.963100000000001</v>
       </c>
       <c r="D19">
         <v>2147225.4</v>
@@ -927,13 +959,13 @@
         <v>3.77</v>
       </c>
       <c r="H19">
-        <v>156022058.57</v>
+        <v>156022058.56999999</v>
       </c>
       <c r="I19">
         <v>154708091.63</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44348</v>
       </c>
@@ -941,13 +973,13 @@
         <v>4.32</v>
       </c>
       <c r="C20">
-        <v>20.0301</v>
+        <v>20.030100000000001</v>
       </c>
       <c r="D20">
         <v>2156047</v>
       </c>
       <c r="E20">
-        <v>4605.3268</v>
+        <v>4605.3267999999998</v>
       </c>
       <c r="F20">
         <v>0.53</v>
@@ -962,21 +994,21 @@
         <v>154902608.69</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44378</v>
       </c>
       <c r="B21">
-        <v>4.52</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="C21">
-        <v>19.9701</v>
+        <v>19.970099999999999</v>
       </c>
       <c r="D21">
         <v>2177779.4</v>
       </c>
       <c r="E21">
-        <v>4616.2582</v>
+        <v>4616.2582000000002</v>
       </c>
       <c r="F21">
         <v>0.59</v>
@@ -985,27 +1017,27 @@
         <v>3.84</v>
       </c>
       <c r="H21">
-        <v>159924496.14</v>
+        <v>159924496.13999999</v>
       </c>
       <c r="I21">
         <v>156602764.72</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44409</v>
       </c>
       <c r="B22">
-        <v>4.65</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="C22">
         <v>20.0761</v>
       </c>
       <c r="D22">
-        <v>2174192.3</v>
+        <v>2174192.2999999998</v>
       </c>
       <c r="E22">
-        <v>4776.7196</v>
+        <v>4776.7196000000004</v>
       </c>
       <c r="F22">
         <v>0.19</v>
@@ -1017,10 +1049,10 @@
         <v>161444186.91</v>
       </c>
       <c r="I22">
-        <v>156601080.6</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>156601080.59999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44440</v>
       </c>
@@ -1034,7 +1066,7 @@
         <v>2198931.1</v>
       </c>
       <c r="E23">
-        <v>4436.0128</v>
+        <v>4436.0128000000004</v>
       </c>
       <c r="F23">
         <v>0.62</v>
@@ -1043,27 +1075,27 @@
         <v>4</v>
       </c>
       <c r="H23">
-        <v>163199015.23</v>
+        <v>163199015.22999999</v>
       </c>
       <c r="I23">
-        <v>160031446.17</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>160031446.16999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44470</v>
       </c>
       <c r="B24">
-        <v>4.98</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="C24">
-        <v>20.4626</v>
+        <v>20.462599999999998</v>
       </c>
       <c r="D24">
-        <v>2225574.3</v>
+        <v>2225574.2999999998</v>
       </c>
       <c r="E24">
-        <v>4854.0866</v>
+        <v>4854.0865999999996</v>
       </c>
       <c r="F24">
         <v>0.84</v>
@@ -1072,13 +1104,13 @@
         <v>4.13</v>
       </c>
       <c r="H24">
-        <v>164597773.65</v>
+        <v>164597773.65000001</v>
       </c>
       <c r="I24">
         <v>159717283.56</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44501</v>
       </c>
@@ -1086,16 +1118,16 @@
         <v>5.13</v>
       </c>
       <c r="C25">
-        <v>20.9004</v>
+        <v>20.900400000000001</v>
       </c>
       <c r="D25">
         <v>2286794.1</v>
       </c>
       <c r="E25">
-        <v>4689.3135</v>
+        <v>4689.3135000000002</v>
       </c>
       <c r="F25">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="G25">
         <v>4.26</v>
@@ -1107,7 +1139,7 @@
         <v>167262488.31</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44531</v>
       </c>
@@ -1118,10 +1150,10 @@
         <v>20.8918</v>
       </c>
       <c r="D26">
-        <v>2440780.7</v>
+        <v>2440780.7000000002</v>
       </c>
       <c r="E26">
-        <v>4767.7923</v>
+        <v>4767.7923000000001</v>
       </c>
       <c r="F26">
         <v>0.36</v>
@@ -1130,13 +1162,13 @@
         <v>4.47</v>
       </c>
       <c r="H26">
-        <v>166946866.98</v>
+        <v>166946866.97999999</v>
       </c>
       <c r="I26">
-        <v>164324562.33</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>164324562.33000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44562</v>
       </c>
@@ -1144,7 +1176,7 @@
         <v>5.72</v>
       </c>
       <c r="C27">
-        <v>20.4978</v>
+        <v>20.497800000000002</v>
       </c>
       <c r="D27">
         <v>2433663.5</v>
@@ -1162,10 +1194,10 @@
         <v>168849200.28</v>
       </c>
       <c r="I27">
-        <v>168063891.7</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>168063891.69999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44593</v>
       </c>
@@ -1179,13 +1211,13 @@
         <v>2438545.9</v>
       </c>
       <c r="E28">
-        <v>3928.4852</v>
+        <v>3928.4852000000001</v>
       </c>
       <c r="F28">
         <v>0.83</v>
       </c>
       <c r="G28">
-        <v>4.85</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="H28">
         <v>169897997.12</v>
@@ -1194,7 +1226,7 @@
         <v>168128795.91</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44621</v>
       </c>
@@ -1205,25 +1237,25 @@
         <v>20.5562</v>
       </c>
       <c r="D29">
-        <v>2511751.2</v>
+        <v>2511751.2000000002</v>
       </c>
       <c r="E29">
-        <v>4712.0937</v>
+        <v>4712.0937000000004</v>
       </c>
       <c r="F29">
         <v>0.99</v>
       </c>
       <c r="G29">
-        <v>5.06</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="H29">
-        <v>171593122.29</v>
+        <v>171593122.28999999</v>
       </c>
       <c r="I29">
-        <v>171262933.29</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>171262933.28999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44652</v>
       </c>
@@ -1231,13 +1263,13 @@
         <v>6.73</v>
       </c>
       <c r="C30">
-        <v>20.1088</v>
+        <v>20.108799999999999</v>
       </c>
       <c r="D30">
         <v>2474416</v>
       </c>
       <c r="E30">
-        <v>4749.1098</v>
+        <v>4749.1098000000002</v>
       </c>
       <c r="F30">
         <v>0.54</v>
@@ -1246,13 +1278,13 @@
         <v>5.35</v>
       </c>
       <c r="H30">
-        <v>172790622.15</v>
+        <v>172790622.15000001</v>
       </c>
       <c r="I30">
         <v>171273558.53</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44682</v>
       </c>
@@ -1263,10 +1295,10 @@
         <v>20.0305</v>
       </c>
       <c r="D31">
-        <v>2463886.2</v>
+        <v>2463886.2000000002</v>
       </c>
       <c r="E31">
-        <v>5173.7153</v>
+        <v>5173.7152999999998</v>
       </c>
       <c r="F31">
         <v>0.18</v>
@@ -1275,13 +1307,13 @@
         <v>5.58</v>
       </c>
       <c r="H31">
-        <v>174141379.01</v>
+        <v>174141379.00999999</v>
       </c>
       <c r="I31">
-        <v>170917406.23</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>170917406.22999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44713</v>
       </c>
@@ -1289,13 +1321,13 @@
         <v>7.42</v>
       </c>
       <c r="C32">
-        <v>20.0237</v>
+        <v>20.023700000000002</v>
       </c>
       <c r="D32">
-        <v>2455161.2</v>
+        <v>2455161.2000000002</v>
       </c>
       <c r="E32">
-        <v>5150.2223</v>
+        <v>5150.2223000000004</v>
       </c>
       <c r="F32">
         <v>0.84</v>
@@ -1304,27 +1336,27 @@
         <v>5.87</v>
       </c>
       <c r="H32">
-        <v>175343664.8</v>
+        <v>175343664.80000001</v>
       </c>
       <c r="I32">
-        <v>171415280.24</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>171415280.24000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44743</v>
       </c>
       <c r="B33">
-        <v>8.039999999999999</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="C33">
-        <v>20.5467</v>
+        <v>20.546700000000001</v>
       </c>
       <c r="D33">
-        <v>2489346.7</v>
+        <v>2489346.7000000002</v>
       </c>
       <c r="E33">
-        <v>5342.837</v>
+        <v>5342.8370000000004</v>
       </c>
       <c r="F33">
         <v>0.74</v>
@@ -1333,13 +1365,13 @@
         <v>6.27</v>
       </c>
       <c r="H33">
-        <v>176901804.9</v>
+        <v>176901804.90000001</v>
       </c>
       <c r="I33">
         <v>174476063.63</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44774</v>
       </c>
@@ -1347,13 +1379,13 @@
         <v>8.5</v>
       </c>
       <c r="C34">
-        <v>20.1209</v>
+        <v>20.120899999999999</v>
       </c>
       <c r="D34">
-        <v>2459987.3</v>
+        <v>2459987.2999999998</v>
       </c>
       <c r="E34">
-        <v>5160.1441</v>
+        <v>5160.1441000000004</v>
       </c>
       <c r="F34">
         <v>0.7</v>
@@ -1362,27 +1394,27 @@
         <v>6.6</v>
       </c>
       <c r="H34">
-        <v>178823724.61</v>
+        <v>178823724.61000001</v>
       </c>
       <c r="I34">
         <v>175097369.81</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44805</v>
       </c>
       <c r="B35">
-        <v>8.890000000000001</v>
+        <v>8.89</v>
       </c>
       <c r="C35">
-        <v>20.075</v>
+        <v>20.074999999999999</v>
       </c>
       <c r="D35">
-        <v>2480963.3</v>
+        <v>2480963.2999999998</v>
       </c>
       <c r="E35">
-        <v>5078.5862</v>
+        <v>5078.5861999999997</v>
       </c>
       <c r="F35">
         <v>0.62</v>
@@ -1391,13 +1423,13 @@
         <v>6.95</v>
       </c>
       <c r="H35">
-        <v>180381442.3</v>
+        <v>180381442.30000001</v>
       </c>
       <c r="I35">
-        <v>180017974.54</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>180017974.53999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44835</v>
       </c>
@@ -1405,16 +1437,16 @@
         <v>9.56</v>
       </c>
       <c r="C36">
-        <v>19.9845</v>
+        <v>19.984500000000001</v>
       </c>
       <c r="D36">
         <v>2492681</v>
       </c>
       <c r="E36">
-        <v>5404.6702</v>
+        <v>5404.6701999999996</v>
       </c>
       <c r="F36">
-        <v>0.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G36">
         <v>7.42</v>
@@ -1423,10 +1455,10 @@
         <v>181978288.34</v>
       </c>
       <c r="I36">
-        <v>179790443.92</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>179790443.91999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44866</v>
       </c>
@@ -1434,16 +1466,16 @@
         <v>10</v>
       </c>
       <c r="C37">
-        <v>19.4449</v>
+        <v>19.444900000000001</v>
       </c>
       <c r="D37">
-        <v>2546233.2</v>
+        <v>2546233.2000000002</v>
       </c>
       <c r="E37">
-        <v>4853.746</v>
+        <v>4853.7460000000001</v>
       </c>
       <c r="F37">
-        <v>0.58</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G37">
         <v>7.79</v>
@@ -1452,10 +1484,10 @@
         <v>182364460.5</v>
       </c>
       <c r="I37">
-        <v>184057953.39</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>184057953.38999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44896</v>
       </c>
@@ -1469,7 +1501,7 @@
         <v>2700041.3</v>
       </c>
       <c r="E38">
-        <v>5379.1316</v>
+        <v>5379.1315999999997</v>
       </c>
       <c r="F38">
         <v>0.38</v>
@@ -1478,13 +1510,13 @@
         <v>8.23</v>
       </c>
       <c r="H38">
-        <v>184558451.54</v>
+        <v>184558451.53999999</v>
       </c>
       <c r="I38">
         <v>185878057.28</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44927</v>
       </c>
@@ -1498,22 +1530,22 @@
         <v>2663290.9</v>
       </c>
       <c r="E39">
-        <v>4434.7719</v>
+        <v>4434.7718999999997</v>
       </c>
       <c r="F39">
         <v>0.68</v>
       </c>
       <c r="G39">
-        <v>8.630000000000001</v>
+        <v>8.6300000000000008</v>
       </c>
       <c r="H39">
-        <v>186293457.2</v>
+        <v>186293457.19999999</v>
       </c>
       <c r="I39">
-        <v>188750112.21</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>188750112.21000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44958</v>
       </c>
@@ -1521,16 +1553,16 @@
         <v>11.1</v>
       </c>
       <c r="C40">
-        <v>18.5986</v>
+        <v>18.598600000000001</v>
       </c>
       <c r="D40">
         <v>2640274.1</v>
       </c>
       <c r="E40">
-        <v>4346.1517</v>
+        <v>4346.1517000000003</v>
       </c>
       <c r="F40">
-        <v>0.5600000000000001</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G40">
         <v>8.93</v>
@@ -1542,7 +1574,7 @@
         <v>189630083.09</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44986</v>
       </c>
@@ -1553,25 +1585,25 @@
         <v>18.3749</v>
       </c>
       <c r="D41">
-        <v>2681153.2</v>
+        <v>2681153.2000000002</v>
       </c>
       <c r="E41">
-        <v>5189.392</v>
+        <v>5189.3919999999998</v>
       </c>
       <c r="F41">
         <v>0.27</v>
       </c>
       <c r="G41">
-        <v>9.199999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="H41">
         <v>188548146.25</v>
       </c>
       <c r="I41">
-        <v>193360881.4</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>193360881.40000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>45017</v>
       </c>
@@ -1585,22 +1617,22 @@
         <v>2662966.5</v>
       </c>
       <c r="E42">
-        <v>5006.8015</v>
+        <v>5006.8014999999996</v>
       </c>
       <c r="F42">
         <v>-0.02</v>
       </c>
       <c r="G42">
-        <v>9.390000000000001</v>
+        <v>9.39</v>
       </c>
       <c r="H42">
-        <v>189619493.93</v>
+        <v>189619493.93000001</v>
       </c>
       <c r="I42">
-        <v>193410033.36</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>193410033.36000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>45047</v>
       </c>
@@ -1608,13 +1640,13 @@
         <v>11.54</v>
       </c>
       <c r="C43">
-        <v>17.7373</v>
+        <v>17.737300000000001</v>
       </c>
       <c r="D43">
         <v>2683963</v>
       </c>
       <c r="E43">
-        <v>5675.8614</v>
+        <v>5675.8613999999998</v>
       </c>
       <c r="F43">
         <v>-0.22</v>
@@ -1623,13 +1655,13 @@
         <v>9.51</v>
       </c>
       <c r="H43">
-        <v>191558644.11</v>
+        <v>191558644.11000001</v>
       </c>
       <c r="I43">
-        <v>197219686.15</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>197219686.15000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>45078</v>
       </c>
@@ -1637,13 +1669,13 @@
         <v>11.5</v>
       </c>
       <c r="C44">
-        <v>17.2412</v>
+        <v>17.241199999999999</v>
       </c>
       <c r="D44">
         <v>2684908.4</v>
       </c>
       <c r="E44">
-        <v>5584.4913</v>
+        <v>5584.4912999999997</v>
       </c>
       <c r="F44">
         <v>0.1</v>
@@ -1655,10 +1687,10 @@
         <v>193309306.59</v>
       </c>
       <c r="I44">
-        <v>196950139.82</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>196950139.81999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>45108</v>
       </c>
@@ -1666,28 +1698,28 @@
         <v>11.5</v>
       </c>
       <c r="C45">
-        <v>16.9049</v>
+        <v>16.904900000000001</v>
       </c>
       <c r="D45">
         <v>2711162</v>
       </c>
       <c r="E45">
-        <v>5668.486</v>
+        <v>5668.4859999999999</v>
       </c>
       <c r="F45">
         <v>0.48</v>
       </c>
       <c r="G45">
-        <v>9.609999999999999</v>
+        <v>9.61</v>
       </c>
       <c r="H45">
-        <v>193759384.18</v>
+        <v>193759384.18000001</v>
       </c>
       <c r="I45">
         <v>200525614</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45139</v>
       </c>
@@ -1695,28 +1727,28 @@
         <v>11.5</v>
       </c>
       <c r="C46">
-        <v>16.9766</v>
+        <v>16.976600000000001</v>
       </c>
       <c r="D46">
         <v>2680309.5</v>
       </c>
       <c r="E46">
-        <v>5568.2516</v>
+        <v>5568.2515999999996</v>
       </c>
       <c r="F46">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G46">
-        <v>9.619999999999999</v>
+        <v>9.6199999999999992</v>
       </c>
       <c r="H46">
-        <v>194244468.74</v>
+        <v>194244468.74000001</v>
       </c>
       <c r="I46">
-        <v>199471548.8</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>199471548.80000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45170</v>
       </c>
@@ -1724,28 +1756,28 @@
         <v>11.5</v>
       </c>
       <c r="C47">
-        <v>17.3077</v>
+        <v>17.307700000000001</v>
       </c>
       <c r="D47">
         <v>2702814.8</v>
       </c>
       <c r="E47">
-        <v>5616.5469</v>
+        <v>5616.5469000000003</v>
       </c>
       <c r="F47">
         <v>0.44</v>
       </c>
       <c r="G47">
-        <v>9.640000000000001</v>
+        <v>9.64</v>
       </c>
       <c r="H47">
-        <v>195894568.85</v>
+        <v>195894568.84999999</v>
       </c>
       <c r="I47">
-        <v>206795396.42</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>206795396.41999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45200</v>
       </c>
@@ -1759,7 +1791,7 @@
         <v>2718500.9</v>
       </c>
       <c r="E48">
-        <v>5817.8255</v>
+        <v>5817.8254999999999</v>
       </c>
       <c r="F48">
         <v>0.38</v>
@@ -1771,10 +1803,10 @@
         <v>197425412.12</v>
       </c>
       <c r="I48">
-        <v>185990915.64</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>185990915.63999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>45231</v>
       </c>
@@ -1788,22 +1820,22 @@
         <v>2780023.7</v>
       </c>
       <c r="E49">
-        <v>4913.0678</v>
+        <v>4913.0677999999998</v>
       </c>
       <c r="F49">
         <v>0.64</v>
       </c>
       <c r="G49">
-        <v>9.710000000000001</v>
+        <v>9.7100000000000009</v>
       </c>
       <c r="H49">
-        <v>198070757.95</v>
+        <v>198070757.94999999</v>
       </c>
       <c r="I49">
         <v>189779599.63</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>45261</v>
       </c>
@@ -1817,7 +1849,7 @@
         <v>2960457.5</v>
       </c>
       <c r="E50">
-        <v>5497.0246</v>
+        <v>5497.0245999999997</v>
       </c>
       <c r="F50">
         <v>0.71</v>
@@ -1826,13 +1858,13 @@
         <v>9.83</v>
       </c>
       <c r="H50">
-        <v>200779197.92</v>
+        <v>200779197.91999999</v>
       </c>
       <c r="I50">
-        <v>188244558.32</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>188244558.31999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>45292</v>
       </c>
@@ -1840,28 +1872,28 @@
         <v>11.5</v>
       </c>
       <c r="C51">
-        <v>17.0873</v>
+        <v>17.087299999999999</v>
       </c>
       <c r="D51">
         <v>2957616</v>
       </c>
       <c r="E51">
-        <v>4573.2226</v>
+        <v>4573.2226000000001</v>
       </c>
       <c r="F51">
         <v>0.89</v>
       </c>
       <c r="G51">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="H51">
-        <v>205156192.79</v>
+        <v>205156192.78999999</v>
       </c>
       <c r="I51">
-        <v>192710166.32</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>192710166.31999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>45323</v>
       </c>
@@ -1875,13 +1907,13 @@
         <v>3013956.6</v>
       </c>
       <c r="E52">
-        <v>4494.8384</v>
+        <v>4494.8383999999996</v>
       </c>
       <c r="F52">
         <v>0.09</v>
       </c>
       <c r="G52">
-        <v>9.859999999999999</v>
+        <v>9.86</v>
       </c>
       <c r="H52">
         <v>209526206.94</v>
@@ -1890,7 +1922,7 @@
         <v>194141036.94</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>45352</v>
       </c>
@@ -1898,28 +1930,28 @@
         <v>11.44</v>
       </c>
       <c r="C53">
-        <v>16.7918</v>
+        <v>16.791799999999999</v>
       </c>
       <c r="D53">
         <v>3043322.6</v>
       </c>
       <c r="E53">
-        <v>5014.5816</v>
+        <v>5014.5816000000004</v>
       </c>
       <c r="F53">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="G53">
-        <v>9.859999999999999</v>
+        <v>9.86</v>
       </c>
       <c r="H53">
-        <v>213910157.18</v>
+        <v>213910157.18000001</v>
       </c>
       <c r="I53">
         <v>200351902.37</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>45383</v>
       </c>
@@ -1927,13 +1959,13 @@
         <v>11.25</v>
       </c>
       <c r="C54">
-        <v>16.8104</v>
+        <v>16.810400000000001</v>
       </c>
       <c r="D54">
         <v>2980374.6</v>
       </c>
       <c r="E54">
-        <v>5418.8526</v>
+        <v>5418.8526000000002</v>
       </c>
       <c r="F54">
         <v>0.2</v>
@@ -1942,13 +1974,13 @@
         <v>9.76</v>
       </c>
       <c r="H54">
-        <v>217234185.04</v>
+        <v>217234185.03999999</v>
       </c>
       <c r="I54">
         <v>197495537.84</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>45413</v>
       </c>
@@ -1956,13 +1988,13 @@
         <v>11.24</v>
       </c>
       <c r="C55">
-        <v>16.7936</v>
+        <v>16.793600000000001</v>
       </c>
       <c r="D55">
         <v>2989794.8</v>
       </c>
       <c r="E55">
-        <v>5618.1155</v>
+        <v>5618.1154999999999</v>
       </c>
       <c r="F55">
         <v>-0.19</v>
@@ -1971,13 +2003,13 @@
         <v>9.73</v>
       </c>
       <c r="H55">
-        <v>225679008.98</v>
+        <v>225679008.97999999</v>
       </c>
       <c r="I55">
         <v>201680789.37</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>45444</v>
       </c>
@@ -1985,13 +2017,13 @@
         <v>11.24</v>
       </c>
       <c r="C56">
-        <v>18.2174</v>
+        <v>18.217400000000001</v>
       </c>
       <c r="D56">
         <v>2995218.5</v>
       </c>
       <c r="E56">
-        <v>6206.8793</v>
+        <v>6206.8792999999996</v>
       </c>
       <c r="F56">
         <v>0.38</v>

</xml_diff>